<commit_message>
Guide to setting up MySQL on Azure
</commit_message>
<xml_diff>
--- a/TermProject/TermProjectProposalRubric_CS295N.xlsx
+++ b/TermProject/TermProjectProposalRubric_CS295N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS295N-CourseMaterials/TermProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2902D2B9-D09F-2F4C-BC02-96240BE3F28B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95797825-61AA-424E-A853-B5A4CDD11797}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>-----------------------------------</t>
   </si>
@@ -56,7 +56,16 @@
     <t>Excellent work! Your proposal looks good and includes all the required details. Your web site should meet all the term project requirements and doesn't look like it would be too difficult. It looks like an interesting and fun site!</t>
   </si>
   <si>
-    <t>(You are being garded on the quality and completeness of the proposal, not on whether the proposed site meets all the requirements for the term project.)</t>
+    <t>Poorly written</t>
+  </si>
+  <si>
+    <t>Not clear, doesn't match UI sketch</t>
+  </si>
+  <si>
+    <t>Not done.</t>
+  </si>
+  <si>
+    <t>Nice!</t>
   </si>
 </sst>
 </file>
@@ -970,15 +979,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="1.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19">
@@ -991,115 +1003,125 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="12"/>
-    </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="6"/>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="18">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
       <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="F7" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>7</v>
+      <c r="A8" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>20</v>
-      </c>
-      <c r="C9">
-        <v>20</v>
-      </c>
-      <c r="F9" s="6"/>
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4">
+        <f>SUM(B5:B8)</f>
+        <v>50</v>
+      </c>
+      <c r="C9" s="4">
+        <f>SUM(C5:C8)</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="4">
-        <f>SUM(B6:B9)</f>
-        <v>50</v>
-      </c>
-      <c r="C10" s="4">
-        <f>SUM(C6:C9)</f>
-        <v>50</v>
-      </c>
+      <c r="A10" s="12"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="12"/>
-      <c r="F11" s="6"/>
+      <c r="A11" s="12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="12"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="12"/>
-      <c r="F13" s="6"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="13"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="12"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="A16" s="8"/>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="8"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6">
+      <c r="A18" s="6"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6">
@@ -1107,52 +1129,51 @@
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="6"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="A21" s="1"/>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="1"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6">
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6">
+      <c r="A25" s="4"/>
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="4"/>
+      <c r="A26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="6"/>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="4"/>
-      <c r="F29" s="6"/>
+    <row r="28" spans="1:6">
+      <c r="A28" s="4"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6">
+      <c r="A31" s="4"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="4"/>
-      <c r="F32" s="6"/>
+    <row r="33" spans="1:6">
+      <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="F34" s="6"/>
+      <c r="A34" s="12"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="12"/>
@@ -1161,62 +1182,59 @@
       <c r="A36" s="12"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="12"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="7"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="8"/>
+      <c r="A39" s="8"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="6"/>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="6"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="6"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+      <c r="A44" s="1"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="1"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="9"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
+      <c r="A46" s="1"/>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="4"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="4"/>
+      <c r="A50" s="1"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="2"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-    </row>
-    <row r="55" spans="1:3" s="4" customFormat="1"/>
+      <c r="A52" s="2"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+    </row>
+    <row r="54" spans="1:3" s="4" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the term project requirements
</commit_message>
<xml_diff>
--- a/TermProject/TermProjectProposalRubric_CS295N.xlsx
+++ b/TermProject/TermProjectProposalRubric_CS295N.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS295N-CourseMaterials/TermProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS295N-CourseMaterials/TermProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95797825-61AA-424E-A853-B5A4CDD11797}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F758706-3482-3040-B303-36617A78FCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27880" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Student Points" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>-----------------------------------</t>
   </si>
@@ -56,16 +69,7 @@
     <t>Excellent work! Your proposal looks good and includes all the required details. Your web site should meet all the term project requirements and doesn't look like it would be too difficult. It looks like an interesting and fun site!</t>
   </si>
   <si>
-    <t>Poorly written</t>
-  </si>
-  <si>
-    <t>Not clear, doesn't match UI sketch</t>
-  </si>
-  <si>
-    <t>Not done.</t>
-  </si>
-  <si>
-    <t>Nice!</t>
+    <t>You are being graded on the quality and completeness of the proposal, not on whether the proposed site meets all the requirements for the term project.</t>
   </si>
 </sst>
 </file>
@@ -622,8 +626,10 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -981,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1008,9 +1014,6 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6">
@@ -1020,12 +1023,6 @@
       <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="6" spans="1:6" ht="18">
       <c r="A6" t="s">
@@ -1034,12 +1031,6 @@
       <c r="B6">
         <v>10</v>
       </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6">
@@ -1049,25 +1040,13 @@
       <c r="B7">
         <v>10</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="12" t="s">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>20</v>
-      </c>
-      <c r="C8">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
       </c>
       <c r="F8" s="6"/>
     </row>
@@ -1079,34 +1058,29 @@
         <f>SUM(B5:B8)</f>
         <v>50</v>
       </c>
-      <c r="C9" s="4">
-        <f>SUM(C5:C8)</f>
-        <v>30</v>
-      </c>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="12"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="12" t="s">
-        <v>9</v>
-      </c>
+    <row r="11" spans="1:6" ht="102" customHeight="1">
+      <c r="A11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="12"/>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="13"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="A13" s="12"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="3"/>
@@ -1172,15 +1146,6 @@
     <row r="33" spans="1:6">
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="12"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="12"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="12"/>
-    </row>
     <row r="37" spans="1:6">
       <c r="A37" s="7"/>
       <c r="B37" s="3"/>
@@ -1236,6 +1201,9 @@
     </row>
     <row r="54" spans="1:3" s="4" customFormat="1"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:D11"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1269,7 +1237,7 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="12" t="s">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1318,7 +1286,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="12" t="s">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -1398,15 +1366,10 @@
     <row r="28" spans="1:6">
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="12"/>
-    </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="12"/>
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="12"/>
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6">

</xml_diff>